<commit_message>
fix: affichage des bonnes stats
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\VBOXSVR\_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90969AD-2428-FF4F-93E8-18E5023386A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="13100" yWindow="500" windowWidth="18680" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -371,10 +372,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -454,15 +454,6 @@
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -483,7 +474,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -512,6 +503,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -860,815 +860,815 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76:C76"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="7" customWidth="1"/>
-    <col min="5" max="1023" width="14.42578125" style="4" customWidth="1"/>
-    <col min="1024" max="1025" width="11.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="4" customWidth="1"/>
+    <col min="5" max="1023" width="14.5" style="1" customWidth="1"/>
+    <col min="1024" max="1025" width="11.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="2:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="8"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="5"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="9" spans="2:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="9" spans="2:4" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="2:4" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
+      <c r="C9" s="22"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="12"/>
+    </row>
+    <row r="11" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
+    <row r="12" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="15" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+    <row r="13" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="20"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B17" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="C17" s="19"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="12"/>
+    </row>
+    <row r="19" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B20" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="C23" s="14"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B24" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="15" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="s">
+    <row r="25" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="15" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
+    <row r="26" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B26" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="15"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="15"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B28" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="C28" s="19"/>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B29" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="15"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
+      <c r="C29" s="19"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B30" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="15"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="20" t="s">
+      <c r="C30" s="19"/>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B31" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="15"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B32" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="15"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="20" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B33" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="15"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="20" t="s">
+      <c r="C33" s="19"/>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B34" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="15"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
+      <c r="C34" s="19"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B35" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="15"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
+      <c r="C35" s="19"/>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B36" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="22"/>
-      <c r="D36" s="15"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="20" t="s">
+      <c r="C36" s="19"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B37" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="22"/>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+      <c r="C37" s="19"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="15"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+      <c r="C38" s="19"/>
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B39" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="20"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="18" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="12"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="17"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="15"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="20" t="s">
+      <c r="C41" s="14"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B42" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="15" t="s">
+      <c r="C42" s="19"/>
+      <c r="D42" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
+    <row r="43" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B43" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="22"/>
-      <c r="D43" s="15" t="s">
+      <c r="C43" s="19"/>
+      <c r="D43" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
+    <row r="44" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B44" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="22"/>
-      <c r="D44" s="15" t="s">
+      <c r="C44" s="19"/>
+      <c r="D44" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="20" t="s">
+    <row r="45" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B45" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="15" t="s">
+      <c r="C45" s="19"/>
+      <c r="D45" s="12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="20" t="s">
+    <row r="46" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B46" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="15" t="s">
+      <c r="C46" s="19"/>
+      <c r="D46" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="20" t="s">
+    <row r="47" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B47" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="22"/>
-      <c r="D47" s="15" t="s">
+      <c r="C47" s="19"/>
+      <c r="D47" s="12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="20" t="s">
+    <row r="48" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B48" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="15"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="20"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="18" t="s">
+      <c r="C48" s="19"/>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="17"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="15"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" s="20" t="s">
+      <c r="C50" s="14"/>
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B51" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="15"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="20" t="s">
+      <c r="C51" s="19"/>
+      <c r="D51" s="12"/>
+    </row>
+    <row r="52" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B52" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="22"/>
-      <c r="D52" s="15"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="20" t="s">
+      <c r="C52" s="19"/>
+      <c r="D52" s="12"/>
+    </row>
+    <row r="53" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B53" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="15"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="20" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="12"/>
+    </row>
+    <row r="54" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="20" t="s">
+      <c r="C54" s="19"/>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B55" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="15"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="20" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="12"/>
+    </row>
+    <row r="56" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B56" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="22"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="20" t="s">
+      <c r="C56" s="19"/>
+      <c r="D56" s="12"/>
+    </row>
+    <row r="57" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B57" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="15"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="20"/>
-      <c r="C58" s="22"/>
-      <c r="D58" s="15"/>
-    </row>
-    <row r="59" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="18" t="s">
+      <c r="C57" s="19"/>
+      <c r="D57" s="12"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="17"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="12"/>
+    </row>
+    <row r="59" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B59" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="15"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="20" t="s">
+      <c r="C59" s="14"/>
+      <c r="D59" s="12"/>
+    </row>
+    <row r="60" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B60" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="15"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="20" t="s">
+      <c r="C60" s="19"/>
+      <c r="D60" s="12"/>
+    </row>
+    <row r="61" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B61" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="15"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="20" t="s">
+      <c r="C61" s="19"/>
+      <c r="D61" s="12"/>
+    </row>
+    <row r="62" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B62" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="15"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="20" t="s">
+      <c r="C62" s="19"/>
+      <c r="D62" s="12"/>
+    </row>
+    <row r="63" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B63" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="15"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="20" t="s">
+      <c r="C63" s="19"/>
+      <c r="D63" s="12"/>
+    </row>
+    <row r="64" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B64" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="15"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="20" t="s">
+      <c r="C64" s="19"/>
+      <c r="D64" s="12"/>
+    </row>
+    <row r="65" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="22"/>
-      <c r="D65" s="15"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B66" s="20" t="s">
+      <c r="C65" s="19"/>
+      <c r="D65" s="12"/>
+    </row>
+    <row r="66" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B66" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="22"/>
-      <c r="D66" s="15"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="20" t="s">
+      <c r="C66" s="19"/>
+      <c r="D66" s="12"/>
+    </row>
+    <row r="67" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B67" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="15"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="20" t="s">
+      <c r="C67" s="19"/>
+      <c r="D67" s="12"/>
+    </row>
+    <row r="68" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B68" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="22"/>
-      <c r="D68" s="15"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="20"/>
-      <c r="C69" s="22"/>
-      <c r="D69" s="15"/>
-    </row>
-    <row r="70" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="18" t="s">
+      <c r="C68" s="19"/>
+      <c r="D68" s="12"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="17"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="12"/>
+    </row>
+    <row r="70" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B70" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="17"/>
-      <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="20" t="s">
+      <c r="C70" s="14"/>
+      <c r="D70" s="12"/>
+    </row>
+    <row r="71" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B71" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="22"/>
-      <c r="D71" s="15"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="20" t="s">
+      <c r="C71" s="19"/>
+      <c r="D71" s="12"/>
+    </row>
+    <row r="72" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B72" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="22"/>
-      <c r="D72" s="15"/>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="20" t="s">
+      <c r="C72" s="19"/>
+      <c r="D72" s="12"/>
+    </row>
+    <row r="73" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B73" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C73" s="22"/>
-      <c r="D73" s="15"/>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B74" s="20" t="s">
+      <c r="C73" s="19"/>
+      <c r="D73" s="12"/>
+    </row>
+    <row r="74" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="22"/>
-      <c r="D74" s="15"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
-      <c r="C75" s="22"/>
-      <c r="D75" s="15"/>
-    </row>
-    <row r="76" spans="2:4" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
+      <c r="C74" s="19"/>
+      <c r="D74" s="12"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="17"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="12"/>
+    </row>
+    <row r="76" spans="2:4" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="2"/>
-      <c r="D76" s="15"/>
-    </row>
-    <row r="77" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B77" s="16"/>
-      <c r="C77" s="22"/>
-      <c r="D77" s="15"/>
-    </row>
-    <row r="78" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="18" t="s">
+      <c r="C76" s="22"/>
+      <c r="D76" s="12"/>
+    </row>
+    <row r="77" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B77" s="13"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="12"/>
+    </row>
+    <row r="78" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B78" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="17"/>
-      <c r="D78" s="15" t="s">
+      <c r="C78" s="14"/>
+      <c r="D78" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="20" t="s">
+    <row r="79" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B79" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="22"/>
-      <c r="D79" s="15" t="s">
+      <c r="C79" s="19"/>
+      <c r="D79" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="20" t="s">
+    <row r="80" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B80" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="22"/>
-      <c r="D80" s="15" t="s">
+      <c r="C80" s="19"/>
+      <c r="D80" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="20" t="s">
+    <row r="81" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B81" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C81" s="22"/>
-      <c r="D81" s="15"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="20"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="15"/>
-    </row>
-    <row r="83" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="18" t="s">
+      <c r="C81" s="19"/>
+      <c r="D81" s="12"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" s="17"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="12"/>
+    </row>
+    <row r="83" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B83" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C83" s="17"/>
-      <c r="D83" s="15" t="s">
+      <c r="C83" s="14"/>
+      <c r="D83" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="18" t="s">
+    <row r="84" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B84" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="17"/>
-      <c r="D84" s="15" t="s">
+      <c r="C84" s="14"/>
+      <c r="D84" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="20" t="s">
+    <row r="85" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B85" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="22"/>
-      <c r="D85" s="15"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="20" t="s">
+      <c r="C85" s="19"/>
+      <c r="D85" s="12"/>
+    </row>
+    <row r="86" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B86" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C86" s="22"/>
-      <c r="D86" s="15"/>
-    </row>
-    <row r="87" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B87" s="20" t="s">
+      <c r="C86" s="19"/>
+      <c r="D86" s="12"/>
+    </row>
+    <row r="87" spans="2:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="B87" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="22"/>
-      <c r="D87" s="15"/>
-    </row>
-    <row r="88" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B88" s="20" t="s">
+      <c r="C87" s="19"/>
+      <c r="D87" s="12"/>
+    </row>
+    <row r="88" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B88" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C88" s="22"/>
-      <c r="D88" s="15"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="20" t="s">
+      <c r="C88" s="19"/>
+      <c r="D88" s="12"/>
+    </row>
+    <row r="89" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B89" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="22"/>
-      <c r="D89" s="15"/>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="20" t="s">
+      <c r="C89" s="19"/>
+      <c r="D89" s="12"/>
+    </row>
+    <row r="90" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B90" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C90" s="22"/>
-      <c r="D90" s="15"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="20" t="s">
+      <c r="C90" s="19"/>
+      <c r="D90" s="12"/>
+    </row>
+    <row r="91" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B91" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="22"/>
-      <c r="D91" s="15"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="20"/>
-      <c r="C92" s="22"/>
-      <c r="D92" s="15"/>
-    </row>
-    <row r="93" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="18" t="s">
+      <c r="C91" s="19"/>
+      <c r="D91" s="12"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B92" s="17"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="12"/>
+    </row>
+    <row r="93" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B93" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C93" s="17"/>
-      <c r="D93" s="15" t="s">
+      <c r="C93" s="14"/>
+      <c r="D93" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="18" t="s">
+    <row r="94" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B94" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="17"/>
-      <c r="D94" s="15" t="s">
+      <c r="C94" s="14"/>
+      <c r="D94" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="20" t="s">
+    <row r="95" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B95" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C95" s="22"/>
-      <c r="D95" s="15"/>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="20" t="s">
+      <c r="C95" s="19"/>
+      <c r="D95" s="12"/>
+    </row>
+    <row r="96" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B96" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C96" s="22"/>
-      <c r="D96" s="15"/>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="20" t="s">
+      <c r="C96" s="19"/>
+      <c r="D96" s="12"/>
+    </row>
+    <row r="97" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B97" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C97" s="22"/>
-      <c r="D97" s="15"/>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="20" t="s">
+      <c r="C97" s="19"/>
+      <c r="D97" s="12"/>
+    </row>
+    <row r="98" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B98" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="22"/>
-      <c r="D98" s="15"/>
-    </row>
-    <row r="99" spans="2:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="18" t="s">
+      <c r="C98" s="19"/>
+      <c r="D98" s="12"/>
+    </row>
+    <row r="99" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B99" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C99" s="17"/>
-      <c r="D99" s="15" t="s">
+      <c r="C99" s="14"/>
+      <c r="D99" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="20" t="s">
+    <row r="100" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B100" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C100" s="22"/>
-      <c r="D100" s="15"/>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="20" t="s">
+      <c r="C100" s="19"/>
+      <c r="D100" s="12"/>
+    </row>
+    <row r="101" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B101" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="22"/>
-      <c r="D101" s="15"/>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="20"/>
-      <c r="C102" s="22"/>
-      <c r="D102" s="15"/>
-    </row>
-    <row r="103" spans="2:4" s="14" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="1" t="s">
+      <c r="C101" s="19"/>
+      <c r="D101" s="12"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B102" s="17"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="12"/>
+    </row>
+    <row r="104" spans="2:4" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C103" s="1"/>
-      <c r="D103" s="15"/>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B104" s="20" t="s">
+      <c r="C104" s="23"/>
+      <c r="D104" s="12"/>
+    </row>
+    <row r="105" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B105" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C104" s="22"/>
-      <c r="D104" s="15"/>
-    </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B105" s="20" t="s">
+      <c r="C105" s="19"/>
+      <c r="D105" s="12"/>
+    </row>
+    <row r="106" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B106" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="C105" s="22"/>
-      <c r="D105" s="15"/>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="20" t="s">
+      <c r="C106" s="19"/>
+      <c r="D106" s="12"/>
+    </row>
+    <row r="107" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B107" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C106" s="22"/>
-      <c r="D106" s="15"/>
-    </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="20" t="s">
+      <c r="C107" s="19"/>
+      <c r="D107" s="12"/>
+    </row>
+    <row r="108" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B108" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C107" s="22"/>
-      <c r="D107" s="15"/>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="20" t="s">
+      <c r="C108" s="19"/>
+      <c r="D108" s="12"/>
+    </row>
+    <row r="109" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B109" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C108" s="22"/>
-      <c r="D108" s="15"/>
-    </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="20" t="s">
+      <c r="C109" s="19"/>
+      <c r="D109" s="12"/>
+    </row>
+    <row r="110" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B110" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C109" s="22"/>
-      <c r="D109" s="15"/>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="20" t="s">
+      <c r="C110" s="19"/>
+      <c r="D110" s="12"/>
+    </row>
+    <row r="111" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C110" s="22"/>
-      <c r="D110" s="15"/>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="20" t="s">
+      <c r="C111" s="19"/>
+      <c r="D111" s="12"/>
+    </row>
+    <row r="112" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B112" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C111" s="22"/>
-      <c r="D111" s="15"/>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="20" t="s">
+      <c r="C112" s="19"/>
+      <c r="D112" s="12"/>
+    </row>
+    <row r="113" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C112" s="22"/>
+      <c r="C113" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix(anonymisation): amélioration des perfs
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90969AD-2428-FF4F-93E8-18E5023386A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B981AABE-3AEF-6540-B1AB-E49C008399C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13100" yWindow="500" windowWidth="18680" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10120" yWindow="500" windowWidth="18680" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -864,7 +864,7 @@
   <dimension ref="A1:AMK113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix(sentry): remise à zéro de Sentry fix(excel): correction d'une donnée manquante dans les exports
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A42315-F26A-DA4A-8461-E600E60DE0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09524F0-C3A2-FE41-ADE7-9AD760EDA348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="760" windowWidth="18680" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>Connexion au portail usager</t>
+  </si>
+  <si>
+    <t>Orientation vers CIAS</t>
+  </si>
+  <si>
+    <t>Autre orientation</t>
   </si>
 </sst>
 </file>
@@ -864,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK114"/>
+  <dimension ref="A1:AMK115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1592,92 +1598,101 @@
       <c r="C101" s="19"/>
       <c r="D101" s="12"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="17"/>
+    <row r="102" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B102" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="C102" s="19"/>
       <c r="D102" s="12"/>
     </row>
-    <row r="104" spans="2:4" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="23" t="s">
+    <row r="103" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B103" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C103" s="19"/>
+      <c r="D103" s="12"/>
+    </row>
+    <row r="105" spans="2:4" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C104" s="23"/>
-      <c r="D104" s="12"/>
-    </row>
-    <row r="105" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B105" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C105" s="19"/>
+      <c r="C105" s="23"/>
       <c r="D105" s="12"/>
     </row>
     <row r="106" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B106" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C106" s="19"/>
       <c r="D106" s="12"/>
     </row>
     <row r="107" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B107" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C107" s="19"/>
       <c r="D107" s="12"/>
     </row>
     <row r="108" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B108" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="12"/>
     </row>
     <row r="109" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="12"/>
     </row>
     <row r="110" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B110" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C110" s="19"/>
       <c r="D110" s="12"/>
     </row>
     <row r="111" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B111" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C111" s="19"/>
       <c r="D111" s="12"/>
     </row>
     <row r="112" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C112" s="19"/>
       <c r="D112" s="12"/>
     </row>
-    <row r="113" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C113" s="19"/>
+      <c r="D113" s="12"/>
+    </row>
+    <row r="114" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C113" s="19"/>
-    </row>
-    <row r="114" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="19"/>
+    </row>
+    <row r="115" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C114" s="19"/>
+      <c r="C115" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
feat(sentry): remise à zéro de Sentry fix(securité): correction de requêtes pour améliorer la sécurité feat(perfs): amélioration de la vérification des données envoyées par l'utilisateur feat(rgaa): mise en conformité de l'outil d'ajout / distribution de courriers feat(docs): ajout de données dans les documents personnalisés feat(procurations): augmentation du nombre de procurations disponibles
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A42315-F26A-DA4A-8461-E600E60DE0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09524F0-C3A2-FE41-ADE7-9AD760EDA348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="760" windowWidth="18680" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>Connexion au portail usager</t>
+  </si>
+  <si>
+    <t>Orientation vers CIAS</t>
+  </si>
+  <si>
+    <t>Autre orientation</t>
   </si>
 </sst>
 </file>
@@ -864,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK114"/>
+  <dimension ref="A1:AMK115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1592,92 +1598,101 @@
       <c r="C101" s="19"/>
       <c r="D101" s="12"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="17"/>
+    <row r="102" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B102" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="C102" s="19"/>
       <c r="D102" s="12"/>
     </row>
-    <row r="104" spans="2:4" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="23" t="s">
+    <row r="103" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B103" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C103" s="19"/>
+      <c r="D103" s="12"/>
+    </row>
+    <row r="105" spans="2:4" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C104" s="23"/>
-      <c r="D104" s="12"/>
-    </row>
-    <row r="105" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B105" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C105" s="19"/>
+      <c r="C105" s="23"/>
       <c r="D105" s="12"/>
     </row>
     <row r="106" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B106" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C106" s="19"/>
       <c r="D106" s="12"/>
     </row>
     <row r="107" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B107" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C107" s="19"/>
       <c r="D107" s="12"/>
     </row>
     <row r="108" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B108" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="12"/>
     </row>
     <row r="109" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B109" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="12"/>
     </row>
     <row r="110" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B110" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C110" s="19"/>
       <c r="D110" s="12"/>
     </row>
     <row r="111" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B111" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C111" s="19"/>
       <c r="D111" s="12"/>
     </row>
     <row r="112" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C112" s="19"/>
       <c r="D112" s="12"/>
     </row>
-    <row r="113" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B113" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C113" s="19"/>
+      <c r="D113" s="12"/>
+    </row>
+    <row r="114" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C113" s="19"/>
-    </row>
-    <row r="114" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B114" s="2" t="s">
+      <c r="C114" s="19"/>
+    </row>
+    <row r="115" spans="2:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C114" s="19"/>
+      <c r="C115" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix(frontend): suppression de pages inutiles fix(api): suppression de code inutile fix(structures): correction d'un bug empêchant la validation du formulaire
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celine.le.ru/Downloads/domifa-master/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09524F0-C3A2-FE41-ADE7-9AD760EDA348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DD36A8-691C-8540-95AD-E32690FB05EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10120" yWindow="760" windowWidth="18680" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -385,41 +396,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4F81BD"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFE46C0A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF4F81BD"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FFE46C0A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -436,6 +416,42 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -461,67 +477,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -870,822 +875,633 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK115"/>
+  <dimension ref="B1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C51" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="4" customWidth="1"/>
-    <col min="5" max="1023" width="14.5" style="1" customWidth="1"/>
-    <col min="1024" max="1025" width="11.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="10" customWidth="1"/>
+    <col min="5" max="1023" width="14.5" customWidth="1"/>
+    <col min="1024" max="1025" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="21"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="5"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10"/>
-    </row>
-    <row r="9" spans="2:4" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="9" spans="2:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="22"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="15" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="12"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="17"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="15" t="s">
+      <c r="C13" s="17"/>
+    </row>
+    <row r="15" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="15" t="s">
+    </row>
+    <row r="19" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="12"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="17"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="15" t="s">
+      <c r="D21" s="11"/>
+    </row>
+    <row r="23" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="12"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="10"/>
     </row>
     <row r="24" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="12"/>
     </row>
     <row r="39" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="17"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B41" s="15" t="s">
+    </row>
+    <row r="41" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="12"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="19"/>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="12"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="17"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="12"/>
-    </row>
-    <row r="50" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B50" s="15" t="s">
+    </row>
+    <row r="50" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="12"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="12"/>
     </row>
     <row r="52" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="12"/>
     </row>
     <row r="53" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="12"/>
     </row>
     <row r="54" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="12"/>
     </row>
     <row r="55" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="12"/>
     </row>
     <row r="56" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="12"/>
     </row>
     <row r="57" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="12"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="17"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="12"/>
-    </row>
-    <row r="59" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B59" s="15" t="s">
+    </row>
+    <row r="59" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B59" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="12"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="10"/>
     </row>
     <row r="60" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="12"/>
     </row>
     <row r="61" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="12"/>
     </row>
     <row r="62" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="12"/>
     </row>
     <row r="63" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="12"/>
     </row>
     <row r="64" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="12"/>
     </row>
     <row r="65" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="12"/>
     </row>
     <row r="66" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="19"/>
-      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C67" s="19"/>
-      <c r="D67" s="12"/>
     </row>
     <row r="68" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="12"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B69" s="17"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="12"/>
-    </row>
-    <row r="70" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B70" s="15" t="s">
+    </row>
+    <row r="70" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B70" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="12"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="10"/>
     </row>
     <row r="71" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="19"/>
-      <c r="D71" s="12"/>
     </row>
     <row r="72" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="19"/>
-      <c r="D72" s="12"/>
     </row>
     <row r="73" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C73" s="19"/>
-      <c r="D73" s="12"/>
     </row>
     <row r="74" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="12"/>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="17"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="12"/>
-    </row>
-    <row r="76" spans="2:4" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="22" t="s">
+    </row>
+    <row r="76" spans="2:4" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="22"/>
-      <c r="D76" s="12"/>
+      <c r="C76" s="6"/>
+      <c r="D76" s="10"/>
     </row>
     <row r="77" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B77" s="13"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="12"/>
-    </row>
-    <row r="78" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B78" s="15" t="s">
+      <c r="B77" s="4"/>
+    </row>
+    <row r="78" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="14"/>
-      <c r="D78" s="12" t="s">
+      <c r="C78" s="15"/>
+      <c r="D78" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="79" spans="2:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="19"/>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="10" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="80" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="81" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C81" s="19"/>
-      <c r="D81" s="12"/>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B82" s="17"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="12"/>
-    </row>
-    <row r="83" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B83" s="15" t="s">
+    </row>
+    <row r="83" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B83" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="12" t="s">
+      <c r="C83" s="15"/>
+      <c r="D83" s="10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="84" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B84" s="15" t="s">
+    <row r="84" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B84" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="12" t="s">
+      <c r="C84" s="15"/>
+      <c r="D84" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="85" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="19"/>
-      <c r="D85" s="12"/>
     </row>
     <row r="86" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C86" s="19"/>
-      <c r="D86" s="12"/>
     </row>
     <row r="87" spans="2:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="19"/>
-      <c r="D87" s="12"/>
     </row>
     <row r="88" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C88" s="19"/>
-      <c r="D88" s="12"/>
     </row>
     <row r="89" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="19"/>
-      <c r="D89" s="12"/>
     </row>
     <row r="90" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C90" s="19"/>
-      <c r="D90" s="12"/>
     </row>
     <row r="91" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="19"/>
-      <c r="D91" s="12"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B92" s="17"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="12"/>
-    </row>
-    <row r="93" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B93" s="15" t="s">
+    </row>
+    <row r="93" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B93" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C93" s="14"/>
-      <c r="D93" s="12" t="s">
+      <c r="C93" s="15"/>
+      <c r="D93" s="10" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B94" s="15" t="s">
+    <row r="94" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B94" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="12" t="s">
+      <c r="C94" s="15"/>
+      <c r="D94" s="10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="95" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C95" s="19"/>
-      <c r="D95" s="12"/>
     </row>
     <row r="96" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C96" s="19"/>
-      <c r="D96" s="12"/>
     </row>
     <row r="97" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C97" s="19"/>
-      <c r="D97" s="12"/>
     </row>
     <row r="98" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C98" s="19"/>
-      <c r="D98" s="12"/>
-    </row>
-    <row r="99" spans="2:4" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B99" s="15" t="s">
+    </row>
+    <row r="99" spans="2:4" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B99" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C99" s="14"/>
-      <c r="D99" s="12" t="s">
+      <c r="C99" s="15"/>
+      <c r="D99" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="100" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B100" s="17" t="s">
+      <c r="B100" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C100" s="19"/>
-      <c r="D100" s="12"/>
     </row>
     <row r="101" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="19"/>
-      <c r="D101" s="12"/>
     </row>
     <row r="102" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C102" s="19"/>
-      <c r="D102" s="12"/>
     </row>
     <row r="103" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C103" s="19"/>
-      <c r="D103" s="12"/>
-    </row>
-    <row r="105" spans="2:4" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="23" t="s">
+    </row>
+    <row r="105" spans="2:4" s="3" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C105" s="23"/>
-      <c r="D105" s="12"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="10"/>
     </row>
     <row r="106" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B106" s="17" t="s">
+      <c r="B106" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C106" s="19"/>
-      <c r="D106" s="12"/>
     </row>
     <row r="107" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B107" s="17" t="s">
+      <c r="B107" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C107" s="19"/>
-      <c r="D107" s="12"/>
     </row>
     <row r="108" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B108" s="17" t="s">
+      <c r="B108" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C108" s="19"/>
-      <c r="D108" s="12"/>
     </row>
     <row r="109" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B109" s="17" t="s">
+      <c r="B109" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C109" s="19"/>
-      <c r="D109" s="12"/>
     </row>
     <row r="110" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B110" s="17" t="s">
+      <c r="B110" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C110" s="19"/>
-      <c r="D110" s="12"/>
     </row>
     <row r="111" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B111" s="17" t="s">
+      <c r="B111" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C111" s="19"/>
-      <c r="D111" s="12"/>
     </row>
     <row r="112" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B112" s="17" t="s">
+      <c r="B112" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C112" s="19"/>
-      <c r="D112" s="12"/>
-    </row>
-    <row r="113" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B113" s="17" t="s">
+    </row>
+    <row r="113" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C113" s="19"/>
-      <c r="D113" s="12"/>
-    </row>
-    <row r="114" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B114" s="17" t="s">
+    </row>
+    <row r="114" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C114" s="19"/>
-    </row>
-    <row r="115" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B115" s="2" t="s">
+    </row>
+    <row r="115" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C115" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
fix(stats): order of stats
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E2B68E-72EC-D34E-AEC6-E1F4C2B386F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10EC534-12AD-7948-A5C0-59B46DA29742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1300" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103:C103"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1118,38 +1118,38 @@
     </row>
     <row r="52" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="14" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="C52" s="4"/>
     </row>
     <row r="53" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="16" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="16" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="16" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="16" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" s="16" t="s">
-        <v>35</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="16" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -1159,94 +1159,94 @@
     </row>
     <row r="61" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="14" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C61" s="4"/>
     </row>
     <row r="62" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="16" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="16" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B64" s="16" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B65" s="16" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="16" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="16" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B69" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B70" s="16" t="s">
-        <v>52</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B70" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="4"/>
     </row>
     <row r="71" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B74" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C74" s="4"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B73" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74" s="16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="75" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="16" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="16" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="16" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="16" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -1261,59 +1261,59 @@
     </row>
     <row r="83" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B83" s="14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C83" s="4"/>
     </row>
     <row r="84" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B84" s="16" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B85" s="16" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B86" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B87" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B89" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C89" s="4"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B88" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B89" s="16" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="90" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B90" s="16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B91" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B92" s="16" t="s">
-        <v>107</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B92" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C92" s="4"/>
     </row>
     <row r="93" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B93" s="16" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B94" s="16" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix(stats): fix excel file
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10EC534-12AD-7948-A5C0-59B46DA29742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5091928D-89D2-884E-9764-C5417573C041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat(stats): add stats in export excel
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5091928D-89D2-884E-9764-C5417573C041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9374AE-13D5-8240-9D1B-8829F7830D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1420" yWindow="980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -380,6 +380,15 @@
   </si>
   <si>
     <t>Axe 2. Activité de domiciliation du JJ/MM/AAAA au JJ/MM/AAAA (en nombre d'actes)</t>
+  </si>
+  <si>
+    <t>Première demande</t>
+  </si>
+  <si>
+    <t>Nombre de domiciliés actifs par type de demande</t>
+  </si>
+  <si>
+    <t>Renouvellement</t>
   </si>
 </sst>
 </file>
@@ -864,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C145"/>
+  <dimension ref="B1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -964,25 +973,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="4"/>
+    <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="16" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B23" s="14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4"/>
     </row>
@@ -996,588 +1004,604 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B26" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="16" t="s">
-        <v>17</v>
-      </c>
+    <row r="27" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B28" s="16" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B29" s="16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="16" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="16" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B41" s="18" t="s">
-        <v>93</v>
+      <c r="B41" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B42" s="16" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B44" s="16" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="16" t="s">
-        <v>97</v>
+      <c r="B45" s="18" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="16" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="16" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B52" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="4"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B51" s="16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B52" s="16" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="53" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B53" s="16" t="s">
-        <v>105</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B55" s="16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B56" s="16" t="s">
-        <v>108</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B56" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="4"/>
     </row>
     <row r="57" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="16" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B61" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="4"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B60" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B61" s="16" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="62" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B62" s="16" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B63" s="16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B64" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B65" s="16" t="s">
-        <v>34</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" s="4"/>
     </row>
     <row r="66" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B70" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C70" s="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B69" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B70" s="16" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="71" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B71" s="16" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B73" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B74" s="16" t="s">
-        <v>49</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C74" s="4"/>
     </row>
     <row r="75" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="16" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="16" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B80" s="16" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B81" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B83" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C83" s="4"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B82" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B83" s="16" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="84" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B84" s="16" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B85" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B86" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B87" s="16" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B87" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" s="4"/>
     </row>
     <row r="88" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B88" s="16" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B89" s="16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B90" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B92" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C92" s="4"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B91" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B92" s="16" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="93" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B93" s="16" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B94" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B96" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C96" s="4"/>
+    </row>
+    <row r="97" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B97" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B98" s="16" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B95" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B96" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B98" s="18" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B99" s="16" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
     </row>
     <row r="100" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B100" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B102" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B103" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B104" s="16" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="101" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B101" s="16" t="s">
+    <row r="105" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B105" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="19" t="s">
+    <row r="107" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C103" s="19"/>
-    </row>
-    <row r="104" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="13"/>
-    </row>
-    <row r="105" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="1" t="s">
+      <c r="C107" s="19"/>
+    </row>
+    <row r="108" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="13"/>
+    </row>
+    <row r="109" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="4"/>
-    </row>
-    <row r="106" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B106" s="16" t="s">
+      <c r="C109" s="4"/>
+    </row>
+    <row r="110" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B110" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B107" s="16" t="s">
+    <row r="111" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="108" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B108" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B110" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C110" s="4"/>
-    </row>
-    <row r="111" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B111" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C111" s="4"/>
     </row>
     <row r="112" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B113" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B114" s="16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B115" s="16" t="s">
-        <v>64</v>
-      </c>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C115" s="4"/>
     </row>
     <row r="116" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B116" s="16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B118" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B119" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B120" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B121" s="16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B118" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C119" s="6"/>
-    </row>
-    <row r="120" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B120" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C120" s="3"/>
-    </row>
-    <row r="121" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B121" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C121" s="3"/>
     </row>
     <row r="122" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B122" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B124" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B125" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B126" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C122" s="6"/>
-    </row>
-    <row r="123" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B123" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C123" s="6"/>
-    </row>
-    <row r="124" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B124" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C124" s="6"/>
-    </row>
-    <row r="125" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B125" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C125" s="6"/>
-    </row>
-    <row r="126" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B126" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C126" s="3"/>
+      <c r="C126" s="6"/>
     </row>
     <row r="127" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B127" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B128" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C128" s="6"/>
     </row>
     <row r="129" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B129" s="16" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="C129" s="6"/>
     </row>
-    <row r="130" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B130" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C130" s="6"/>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B130" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B131" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="C131" s="6"/>
     </row>
-    <row r="132" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B132" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C132" s="20"/>
+    <row r="132" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B132" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C132" s="6"/>
     </row>
     <row r="133" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B133" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C133" s="6"/>
     </row>
     <row r="134" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B134" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C134" s="6"/>
     </row>
-    <row r="135" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B135" s="16" t="s">
-        <v>75</v>
-      </c>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C135" s="6"/>
     </row>
-    <row r="136" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B136" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C136" s="6"/>
+    <row r="136" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C136" s="20"/>
     </row>
     <row r="137" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C137" s="6"/>
     </row>
     <row r="138" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C143" s="6"/>
+    </row>
+    <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B144" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C144" s="6"/>
+    </row>
+    <row r="145" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B145" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C145" s="6"/>
+    </row>
+    <row r="146" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B146" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C146" s="6"/>
+    </row>
+    <row r="147" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B147" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C143" s="6"/>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C144" s="6"/>
-    </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C145" s="6"/>
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C149" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B136:C136"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix(stats): add stats to export
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9374AE-13D5-8240-9D1B-8829F7830D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F4E510-BD51-9342-A1E2-E36B10DAC72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17580" yWindow="-24980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>Renouvellement</t>
+  </si>
+  <si>
+    <t>Colis rééxpédiés</t>
+  </si>
+  <si>
+    <t>Courriers réexpédiés</t>
+  </si>
+  <si>
+    <t>Avis de passage réexpédiés</t>
   </si>
 </sst>
 </file>
@@ -873,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C149"/>
+  <dimension ref="B1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1545,57 +1554,75 @@
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="16" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" s="16" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B144" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C144" s="6"/>
     </row>
     <row r="145" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="16" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C145" s="6"/>
     </row>
     <row r="146" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B146" s="16" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="C146" s="6"/>
     </row>
     <row r="147" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B147" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C147" s="6"/>
+    </row>
+    <row r="148" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B148" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B149" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B150" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C147" s="6"/>
-    </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C148" s="6"/>
-    </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C149" s="6"/>
+      <c r="C150" s="6"/>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C152" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
fix(stats): add new age range
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F4E510-BD51-9342-A1E2-E36B10DAC72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA70E84-869B-9F43-B058-7C8F4CE61AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17580" yWindow="-24980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="115">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -82,18 +82,6 @@
   </si>
   <si>
     <t>Nombre de domiciliés actifs par tranche d'âge</t>
-  </si>
-  <si>
-    <t>Moins de 15 ans</t>
-  </si>
-  <si>
-    <t>15-19 ans</t>
-  </si>
-  <si>
-    <t>20-24 ans</t>
-  </si>
-  <si>
-    <t>25-29 ans</t>
   </si>
   <si>
     <t>30-34 ans</t>
@@ -398,6 +386,12 @@
   </si>
   <si>
     <t>Avis de passage réexpédiés</t>
+  </si>
+  <si>
+    <t>26-29 ans</t>
+  </si>
+  <si>
+    <t>18-25 ans</t>
   </si>
 </sst>
 </file>
@@ -882,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C152"/>
+  <dimension ref="B1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="E129" sqref="E129"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -940,7 +934,7 @@
     </row>
     <row r="9" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C9" s="19"/>
     </row>
@@ -984,17 +978,17 @@
     </row>
     <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1031,604 +1025,594 @@
     </row>
     <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B32" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B33" s="16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B34" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B35" s="16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B36" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B37" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B38" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B39" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B40" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B41" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B42" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B43" s="16" t="s">
-        <v>29</v>
+      <c r="B43" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="B44" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="18" t="s">
-        <v>93</v>
+      <c r="B45" s="16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="16" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="14" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B53" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B54" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B56" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="4"/>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B55" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B56" s="16" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="57" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="16" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B61" s="16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B62" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B63" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B65" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65" s="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B63" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B64" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B65" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="66" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B70" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B71" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B72" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B74" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C74" s="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B72" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" s="4"/>
+    </row>
+    <row r="73" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B73" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B74" s="16" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="75" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="16" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B80" s="16" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B81" s="16" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B82" s="16" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B83" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B84" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B85" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B87" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C87" s="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B85" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B86" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B87" s="16" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="88" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B88" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B89" s="16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B90" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B91" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B93" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B94" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B96" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C96" s="4"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B94" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B95" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B96" s="16" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="97" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B97" s="16" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B98" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B99" s="16" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="100" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B100" s="16" t="s">
-        <v>37</v>
+      <c r="B100" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B101" s="16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B102" s="18" t="s">
-        <v>90</v>
+      <c r="B102" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B103" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B104" s="16" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B105" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C107" s="19"/>
-    </row>
-    <row r="108" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="13"/>
-    </row>
-    <row r="109" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C109" s="4"/>
-    </row>
-    <row r="110" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C105" s="19"/>
+    </row>
+    <row r="106" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="13"/>
+    </row>
+    <row r="107" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C107" s="4"/>
+    </row>
+    <row r="108" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B108" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B109" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B110" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B112" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" s="4"/>
+    </row>
+    <row r="113" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="111" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B111" s="16" t="s">
+      <c r="C113" s="4"/>
+    </row>
+    <row r="114" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B112" s="16" t="s">
+    <row r="115" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B114" s="14" t="s">
+    <row r="116" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B116" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="C114" s="4"/>
-    </row>
-    <row r="115" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B115" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C115" s="4"/>
-    </row>
-    <row r="116" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B116" s="16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B118" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="119" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B119" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B120" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C121" s="6"/>
+    </row>
+    <row r="122" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B122" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B123" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B124" s="16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="121" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B121" s="16" t="s">
+      <c r="C124" s="6"/>
+    </row>
+    <row r="125" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B125" s="16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="122" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B122" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C123" s="6"/>
-    </row>
-    <row r="124" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B124" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C124" s="3"/>
-    </row>
-    <row r="125" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B125" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C125" s="3"/>
+      <c r="C125" s="6"/>
     </row>
     <row r="126" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B126" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C126" s="6"/>
     </row>
     <row r="127" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B127" s="16" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C127" s="6"/>
     </row>
-    <row r="128" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B128" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C128" s="6"/>
+    <row r="128" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B128" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C128" s="3"/>
     </row>
     <row r="129" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B129" s="16" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C129" s="6"/>
     </row>
-    <row r="130" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B130" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C130" s="3"/>
+    <row r="130" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B130" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C130" s="6"/>
     </row>
     <row r="131" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B131" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C131" s="6"/>
     </row>
     <row r="132" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B132" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C132" s="6"/>
     </row>
-    <row r="133" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B133" s="16" t="s">
-        <v>78</v>
-      </c>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C133" s="6"/>
     </row>
-    <row r="134" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B134" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C134" s="6"/>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B134" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C134" s="20"/>
+    </row>
+    <row r="135" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B135" s="16" t="s">
+        <v>76</v>
+      </c>
       <c r="C135" s="6"/>
     </row>
-    <row r="136" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C136" s="20"/>
+    <row r="136" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B136" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C136" s="6"/>
     </row>
     <row r="137" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="16" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C137" s="6"/>
     </row>
     <row r="138" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="16" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="16" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="16" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" s="16" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B144" s="16" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="C144" s="6"/>
     </row>
     <row r="145" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C145" s="6"/>
     </row>
     <row r="146" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B146" s="16" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="C146" s="6"/>
     </row>
     <row r="147" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B147" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B148" s="16" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="C148" s="6"/>
     </row>
-    <row r="149" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B149" s="16" t="s">
-        <v>87</v>
-      </c>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C149" s="6"/>
     </row>
-    <row r="150" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B150" s="16" t="s">
-        <v>77</v>
-      </c>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C150" s="6"/>
-    </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C151" s="6"/>
-    </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C152" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B134:C134"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
feat(stats): add new stats for 'raison de la demande'
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA70E84-869B-9F43-B058-7C8F4CE61AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA3A9F1-60A9-3E4D-8B3A-F25137BF0EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17580" yWindow="-24980" windowWidth="23980" windowHeight="21360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12980" yWindow="-21100" windowWidth="23980" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -392,6 +392,12 @@
   </si>
   <si>
     <t>18-25 ans</t>
+  </si>
+  <si>
+    <t>Lutte contre toute forme de violence (mise à l'abri)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercice d'une activité professionnelle </t>
   </si>
 </sst>
 </file>
@@ -876,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C150"/>
+  <dimension ref="B1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1333,286 +1339,296 @@
         <v>51</v>
       </c>
     </row>
-    <row r="97" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B97" s="16" t="s">
-        <v>40</v>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B97" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B98" s="16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B99" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B100" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="100" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B100" s="18" t="s">
+    <row r="102" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B102" s="18" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B101" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B102" s="16" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B103" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B104" s="16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B105" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="19" t="s">
+    <row r="107" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C105" s="19"/>
-    </row>
-    <row r="106" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="13"/>
-    </row>
-    <row r="107" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="1" t="s">
+      <c r="C107" s="19"/>
+    </row>
+    <row r="108" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="13"/>
+    </row>
+    <row r="109" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C107" s="4"/>
-    </row>
-    <row r="108" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B108" s="16" t="s">
+      <c r="C109" s="4"/>
+    </row>
+    <row r="110" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B110" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="109" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B109" s="16" t="s">
+    <row r="111" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B111" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="110" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B110" s="16" t="s">
+    <row r="112" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B112" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="112" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B112" s="14" t="s">
+    <row r="114" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B114" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C112" s="4"/>
-    </row>
-    <row r="113" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B113" s="14" t="s">
+      <c r="C114" s="4"/>
+    </row>
+    <row r="115" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C113" s="4"/>
-    </row>
-    <row r="114" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B114" s="16" t="s">
+      <c r="C115" s="4"/>
+    </row>
+    <row r="116" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116" s="16" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="115" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B115" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="116" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B116" s="16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="117" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B118" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="119" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B119" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B120" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B121" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B122" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C121" s="6"/>
-    </row>
-    <row r="122" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B122" s="14" t="s">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C123" s="6"/>
+    </row>
+    <row r="124" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B124" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C122" s="3"/>
-    </row>
-    <row r="123" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B123" s="14" t="s">
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B125" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C123" s="3"/>
-    </row>
-    <row r="124" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B124" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C124" s="6"/>
-    </row>
-    <row r="125" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B125" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C125" s="6"/>
+      <c r="C125" s="3"/>
     </row>
     <row r="126" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B126" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C126" s="6"/>
     </row>
     <row r="127" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B127" s="16" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C127" s="6"/>
     </row>
-    <row r="128" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B128" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C128" s="3"/>
+    <row r="128" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B128" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C128" s="6"/>
     </row>
     <row r="129" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B129" s="16" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C129" s="6"/>
     </row>
-    <row r="130" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B130" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C130" s="6"/>
+    <row r="130" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B130" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C130" s="3"/>
     </row>
     <row r="131" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B131" s="16" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C131" s="6"/>
     </row>
     <row r="132" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B132" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C132" s="6"/>
+    </row>
+    <row r="133" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B133" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C133" s="6"/>
+    </row>
+    <row r="134" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B134" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C132" s="6"/>
-    </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C133" s="6"/>
-    </row>
-    <row r="134" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B134" s="20" t="s">
+      <c r="C134" s="6"/>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C135" s="6"/>
+    </row>
+    <row r="136" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C134" s="20"/>
-    </row>
-    <row r="135" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B135" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C135" s="6"/>
-    </row>
-    <row r="136" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B136" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C136" s="6"/>
+      <c r="C136" s="20"/>
     </row>
     <row r="137" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B137" s="16" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C137" s="6"/>
     </row>
     <row r="138" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="16" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="16" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="16" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" s="16" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B144" s="16" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C144" s="6"/>
     </row>
     <row r="145" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C145" s="6"/>
     </row>
     <row r="146" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B146" s="16" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="C146" s="6"/>
     </row>
     <row r="147" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B147" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B148" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C148" s="6"/>
+    </row>
+    <row r="149" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B149" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C149" s="6"/>
+    </row>
+    <row r="150" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B150" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C148" s="6"/>
-    </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C149" s="6"/>
-    </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C150" s="6"/>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C151" s="6"/>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C152" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B136:C136"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix(stats): add new stats items
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA3A9F1-60A9-3E4D-8B3A-F25137BF0EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE7461E-A443-A24F-9370-3701B6C6455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12980" yWindow="-21100" windowWidth="23980" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
   <si>
     <t>Nom de la structure</t>
   </si>
@@ -141,21 +141,12 @@
     <t>Situation résidentielle</t>
   </si>
   <si>
-    <t>Domicile mobile (ex: caravane)</t>
-  </si>
-  <si>
-    <t>Hébergement social (sans service courrier)</t>
-  </si>
-  <si>
     <t>Hébergé chez un tiers</t>
   </si>
   <si>
     <t>Hôtel</t>
   </si>
   <si>
-    <t>Sans abris / Squat</t>
-  </si>
-  <si>
     <t>Autre</t>
   </si>
   <si>
@@ -169,9 +160,6 @@
   </si>
   <si>
     <t>Hébergé, mais ne peut justifier d'une adresse</t>
-  </si>
-  <si>
-    <t>Personnes itinérantes</t>
   </si>
   <si>
     <t xml:space="preserve">Rupture familiale et/ou conjugale </t>
@@ -398,6 +386,21 @@
   </si>
   <si>
     <t xml:space="preserve">Exercice d'une activité professionnelle </t>
+  </si>
+  <si>
+    <t>Sans abris / Squat / Bidonville</t>
+  </si>
+  <si>
+    <t>Domicile mobile (ex: Caravane) / Aire des gens du voyages / habitat itinérant</t>
+  </si>
+  <si>
+    <t>Logement avec impossibilité d'utiliser son adresse</t>
+  </si>
+  <si>
+    <t>Hébergement social stable</t>
+  </si>
+  <si>
+    <t>Mode de vie (itinérants, gens du voyage)</t>
   </si>
 </sst>
 </file>
@@ -882,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C152"/>
+  <dimension ref="B1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -940,7 +943,7 @@
     </row>
     <row r="9" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C9" s="19"/>
     </row>
@@ -984,17 +987,17 @@
     </row>
     <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="18" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B21" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -1031,12 +1034,12 @@
     </row>
     <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B30" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B31" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -1091,47 +1094,47 @@
     </row>
     <row r="43" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -1141,38 +1144,38 @@
     </row>
     <row r="54" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B54" s="14" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B55" s="16" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B56" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B57" s="16" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B58" s="16" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B59" s="16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B60" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -1223,58 +1226,58 @@
     </row>
     <row r="72" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B72" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C72" s="4"/>
     </row>
     <row r="73" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B73" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B74" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B75" s="16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B76" s="16" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B77" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B78" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B79" s="16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B80" s="16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B81" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B82" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="16" x14ac:dyDescent="0.2">
@@ -1290,345 +1293,350 @@
     </row>
     <row r="86" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B86" s="16" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B87" s="16" t="s">
-        <v>36</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B88" s="16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B89" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B90" s="16" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B91" s="16" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B92" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B93" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="94" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B94" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C94" s="4"/>
-    </row>
-    <row r="95" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B95" s="16" t="s">
-        <v>50</v>
-      </c>
+    <row r="95" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B95" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C95" s="4"/>
     </row>
     <row r="96" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B96" s="16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B97" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B98" s="16" t="s">
-        <v>115</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B97" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B98" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B99" s="16" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
     </row>
     <row r="100" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B100" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B101" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="102" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B102" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
     <row r="103" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B103" s="16" t="s">
-        <v>87</v>
+      <c r="B103" s="18" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B104" s="16" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B105" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B106" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C107" s="19"/>
-    </row>
-    <row r="108" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="13"/>
-    </row>
-    <row r="109" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C109" s="4"/>
-    </row>
-    <row r="110" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B110" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="111" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:3" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C108" s="19"/>
+    </row>
+    <row r="109" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="13"/>
+    </row>
+    <row r="110" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C110" s="4"/>
+    </row>
+    <row r="111" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B111" s="16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B112" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B114" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C114" s="4"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B113" s="16" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="115" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B115" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C115" s="4"/>
     </row>
-    <row r="116" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B116" s="16" t="s">
-        <v>57</v>
-      </c>
+    <row r="116" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" s="4"/>
     </row>
     <row r="117" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B117" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B118" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B119" s="16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="120" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B120" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B121" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B122" s="16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C123" s="6"/>
-    </row>
-    <row r="124" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B124" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C124" s="3"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B123" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C124" s="6"/>
     </row>
     <row r="125" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B125" s="14" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C125" s="3"/>
     </row>
-    <row r="126" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B126" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C126" s="6"/>
+    <row r="126" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B126" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C126" s="3"/>
     </row>
     <row r="127" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B127" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B128" s="16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C128" s="6"/>
     </row>
     <row r="129" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B129" s="16" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="C129" s="6"/>
     </row>
-    <row r="130" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B130" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C130" s="3"/>
-    </row>
-    <row r="131" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B131" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C131" s="6"/>
+    <row r="130" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B130" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C130" s="6"/>
+    </row>
+    <row r="131" spans="2:3" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B131" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C131" s="3"/>
     </row>
     <row r="132" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B132" s="16" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C132" s="6"/>
     </row>
     <row r="133" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B133" s="16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C133" s="6"/>
     </row>
     <row r="134" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B134" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C134" s="6"/>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B135" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="C135" s="6"/>
     </row>
-    <row r="136" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B136" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C136" s="20"/>
-    </row>
-    <row r="137" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B137" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C137" s="6"/>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C136" s="6"/>
+    </row>
+    <row r="137" spans="2:3" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C137" s="20"/>
     </row>
     <row r="138" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B138" s="16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="16" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="16" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" s="16" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B144" s="16" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="C144" s="6"/>
     </row>
     <row r="145" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="16" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C145" s="6"/>
     </row>
     <row r="146" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B146" s="16" t="s">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="C146" s="6"/>
     </row>
     <row r="147" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B147" s="16" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B148" s="16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C148" s="6"/>
     </row>
     <row r="149" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B149" s="16" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C149" s="6"/>
     </row>
     <row r="150" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B150" s="16" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C150" s="6"/>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B151" s="16" t="s">
+        <v>69</v>
+      </c>
       <c r="C151" s="6"/>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.2">
       <c r="C152" s="6"/>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C153" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B137:C137"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix(backend): fix export column's order
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE7461E-A443-A24F-9370-3701B6C6455C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D31BF66-FA01-4F4F-97EA-5F6359EC789E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12980" yWindow="-21100" windowWidth="23980" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13900" yWindow="760" windowWidth="20660" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats structure" sheetId="1" r:id="rId1"/>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1550,37 +1550,37 @@
     </row>
     <row r="139" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B139" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B140" s="16" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B141" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B142" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B143" s="16" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B144" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C144" s="6"/>
     </row>

</xml_diff>

<commit_message>
fix(frontend): fix unit tests for referrers
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-stats.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F996FBB-47E3-9E48-A101-DB74CFEDEC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE7C662-D003-D649-8FE3-84E298287DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,9 +410,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -486,30 +483,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -519,15 +498,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -537,17 +510,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,764 +884,750 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109:C136"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="60.83203125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="28.83203125" style="4" customWidth="1"/>
-    <col min="4" max="1022" width="14.5" style="8" customWidth="1"/>
-    <col min="1023" max="1024" width="11.5" style="8" customWidth="1"/>
-    <col min="1025" max="16384" width="8.83203125" style="8"/>
+    <col min="1" max="1" width="2.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="60.83203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="28.83203125" style="12" customWidth="1"/>
+    <col min="4" max="1022" width="14.5" style="4" customWidth="1"/>
+    <col min="1023" max="1024" width="11.5" style="4" customWidth="1"/>
+    <col min="1025" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="17"/>
     </row>
     <row r="5" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="17"/>
     </row>
     <row r="6" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="17"/>
     </row>
     <row r="7" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="9" spans="2:3" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="18" t="s">
+      <c r="C7" s="17"/>
+    </row>
+    <row r="9" spans="2:3" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="18"/>
-    </row>
-    <row r="10" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="12"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="6"/>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="16"/>
-    </row>
-    <row r="15" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="13" t="s">
+      <c r="C13" s="19"/>
+    </row>
+    <row r="15" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B15" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B23" s="13" t="s">
+    <row r="23" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B27" s="13" t="s">
+    <row r="27" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="8" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="9" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="8" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B54" s="13" t="s">
+    <row r="54" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C54" s="3"/>
+      <c r="C54" s="13"/>
     </row>
     <row r="55" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B57" s="15" t="s">
+      <c r="B57" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B63" s="13" t="s">
+    <row r="63" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B63" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="3"/>
+      <c r="C63" s="13"/>
     </row>
     <row r="64" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B66" s="15" t="s">
+      <c r="B66" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B67" s="15" t="s">
+      <c r="B67" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B70" s="15" t="s">
+      <c r="B70" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="72" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B72" s="13" t="s">
+    <row r="72" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B72" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C72" s="3"/>
+      <c r="C72" s="13"/>
     </row>
     <row r="73" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B75" s="15" t="s">
+      <c r="B75" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B77" s="15" t="s">
+      <c r="B77" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B78" s="15" t="s">
+      <c r="B78" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B79" s="15" t="s">
+      <c r="B79" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B81" s="15" t="s">
+      <c r="B81" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="8" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B85" s="13" t="s">
+    <row r="85" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B85" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C85" s="3"/>
+      <c r="C85" s="13"/>
     </row>
     <row r="86" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B86" s="15" t="s">
+      <c r="B86" s="8" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B87" s="15" t="s">
+      <c r="B87" s="8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B88" s="15" t="s">
+      <c r="B88" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B89" s="15" t="s">
+      <c r="B89" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B90" s="15" t="s">
+      <c r="B90" s="8" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="8" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B95" s="13" t="s">
+    <row r="95" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B95" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C95" s="3"/>
+      <c r="C95" s="13"/>
     </row>
     <row r="96" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B96" s="15" t="s">
+      <c r="B96" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="97" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B98" s="8" t="s">
+      <c r="B98" s="4" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="8" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="100" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="101" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B106" s="15" t="s">
+      <c r="B106" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="108" spans="2:3" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="18" t="s">
+    <row r="108" spans="2:3" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B108" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C108" s="18"/>
+      <c r="C108" s="10"/>
     </row>
     <row r="109" spans="2:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="12"/>
-      <c r="C109" s="21"/>
+      <c r="B109" s="6"/>
     </row>
     <row r="110" spans="2:3" s="2" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C110" s="22"/>
+      <c r="C110" s="13"/>
     </row>
     <row r="111" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C111" s="21"/>
     </row>
     <row r="112" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C112" s="21"/>
     </row>
     <row r="113" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C113" s="21"/>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C114" s="21"/>
-    </row>
-    <row r="115" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B115" s="13" t="s">
+    </row>
+    <row r="115" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B115" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C115" s="22"/>
-    </row>
-    <row r="116" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B116" s="13" t="s">
+      <c r="C115" s="13"/>
+    </row>
+    <row r="116" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B116" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C116" s="22"/>
+      <c r="C116" s="13"/>
     </row>
     <row r="117" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C117" s="21"/>
     </row>
     <row r="118" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C118" s="21"/>
     </row>
     <row r="119" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C119" s="21"/>
     </row>
     <row r="120" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C120" s="21"/>
     </row>
     <row r="121" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B121" s="15" t="s">
+      <c r="B121" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C121" s="21"/>
     </row>
     <row r="122" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C122" s="21"/>
     </row>
     <row r="123" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C123" s="21"/>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C124" s="20"/>
-    </row>
-    <row r="125" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B125" s="13" t="s">
+      <c r="C124" s="14"/>
+    </row>
+    <row r="125" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B125" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C125" s="23"/>
-    </row>
-    <row r="126" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B126" s="13" t="s">
+      <c r="C125" s="15"/>
+    </row>
+    <row r="126" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B126" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C126" s="23"/>
+      <c r="C126" s="15"/>
     </row>
     <row r="127" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B127" s="15" t="s">
+      <c r="B127" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C127" s="20"/>
+      <c r="C127" s="14"/>
     </row>
     <row r="128" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B128" s="15" t="s">
+      <c r="B128" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C128" s="20"/>
+      <c r="C128" s="14"/>
     </row>
     <row r="129" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B129" s="15" t="s">
+      <c r="B129" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C129" s="20"/>
+      <c r="C129" s="14"/>
     </row>
     <row r="130" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B130" s="15" t="s">
+      <c r="B130" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C130" s="20"/>
-    </row>
-    <row r="131" spans="2:3" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="B131" s="13" t="s">
+      <c r="C130" s="14"/>
+    </row>
+    <row r="131" spans="2:3" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="B131" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C131" s="23"/>
+      <c r="C131" s="15"/>
     </row>
     <row r="132" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B132" s="15" t="s">
+      <c r="B132" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C132" s="20"/>
+      <c r="C132" s="14"/>
     </row>
     <row r="133" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B133" s="15" t="s">
+      <c r="B133" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C133" s="20"/>
+      <c r="C133" s="14"/>
     </row>
     <row r="134" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B134" s="15" t="s">
+      <c r="B134" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C134" s="20"/>
+      <c r="C134" s="14"/>
     </row>
     <row r="135" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B135" s="15" t="s">
+      <c r="B135" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C135" s="20"/>
+      <c r="C135" s="14"/>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C136" s="20"/>
-    </row>
-    <row r="137" spans="2:3" s="11" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B137" s="19" t="s">
+      <c r="C136" s="14"/>
+    </row>
+    <row r="137" spans="2:3" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C137" s="19"/>
+      <c r="C137" s="11"/>
     </row>
     <row r="138" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B138" s="15" t="s">
+      <c r="B138" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C138" s="20"/>
+      <c r="C138" s="14"/>
     </row>
     <row r="139" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B139" s="15" t="s">
+      <c r="B139" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C139" s="20"/>
+      <c r="C139" s="14"/>
     </row>
     <row r="140" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B140" s="15" t="s">
+      <c r="B140" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C140" s="20"/>
+      <c r="C140" s="14"/>
     </row>
     <row r="141" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B141" s="15" t="s">
+      <c r="B141" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C141" s="20"/>
+      <c r="C141" s="14"/>
     </row>
     <row r="142" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B142" s="15" t="s">
+      <c r="B142" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C142" s="20"/>
+      <c r="C142" s="14"/>
     </row>
     <row r="143" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C143" s="20"/>
+      <c r="C143" s="14"/>
     </row>
     <row r="144" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B144" s="15" t="s">
+      <c r="B144" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C144" s="20"/>
+      <c r="C144" s="14"/>
     </row>
     <row r="145" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B145" s="15" t="s">
+      <c r="B145" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C145" s="20"/>
+      <c r="C145" s="14"/>
     </row>
     <row r="146" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B146" s="15" t="s">
+      <c r="B146" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C146" s="20"/>
+      <c r="C146" s="14"/>
     </row>
     <row r="147" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B147" s="15" t="s">
+      <c r="B147" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C147" s="20"/>
+      <c r="C147" s="14"/>
     </row>
     <row r="148" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B148" s="15" t="s">
+      <c r="B148" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C148" s="20"/>
+      <c r="C148" s="14"/>
     </row>
     <row r="149" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B149" s="15" t="s">
+      <c r="B149" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C149" s="20"/>
+      <c r="C149" s="14"/>
     </row>
     <row r="150" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B150" s="15" t="s">
+      <c r="B150" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C150" s="20"/>
+      <c r="C150" s="14"/>
     </row>
     <row r="151" spans="2:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="B151" s="15" t="s">
+      <c r="B151" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C151" s="20"/>
+      <c r="C151" s="14"/>
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C152" s="5"/>
+      <c r="C152" s="14"/>
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C153" s="5"/>
+      <c r="C153" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>